<commit_message>
identify rows and columns
</commit_message>
<xml_diff>
--- a/input/DOE21E/c133/Std140_HE_Output.xlsx
+++ b/input/DOE21E/c133/Std140_HE_Output.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\DOE21E\c133\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{247C67CE-9DC9-4A29-82A4-7B750207B5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74069ED4-512F-42CF-8642-2EB578E55DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33270" yWindow="2520" windowWidth="25545" windowHeight="20520" xr2:uid="{EA9C7F46-4394-4544-8278-424126D06290}"/>
+    <workbookView xWindow="15255" yWindow="900" windowWidth="25545" windowHeight="20520" xr2:uid="{EA9C7F46-4394-4544-8278-424126D06290}"/>
   </bookViews>
   <sheets>
-    <sheet name="DOE21E" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
   </definedNames>
@@ -400,51 +397,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Read Me"/>
-      <sheetName val="Adding Results"/>
-      <sheetName val="YourData"/>
-      <sheetName val="Title Page"/>
-      <sheetName val="Program List"/>
-      <sheetName val="Table&amp;Figure List"/>
-      <sheetName val="Tables"/>
-      <sheetName val="Fig B16.6-1 LOAD"/>
-      <sheetName val="Fig B16.6-2 INPUT"/>
-      <sheetName val="Fig B16.6-3 FUEL"/>
-      <sheetName val="Fig B16.6-4 FANS"/>
-      <sheetName val="Fig B16.6-5 MEAN T"/>
-      <sheetName val="Fig B16.6-6 MAX T"/>
-      <sheetName val="Fig B16.6-7 MIN T"/>
-      <sheetName val="A"/>
-      <sheetName val="Q-Chart Data"/>
-      <sheetName val="ESP-HOT"/>
-      <sheetName val="EnergyPlusV10"/>
-      <sheetName val="DOE21E"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>